<commit_message>
✨ feat(examples): add script to check and display Excel data   - introduce a Python script to check and display contents of source Excel file   - support CustomerData and Transactions sheets with headers and sample rows
♻️ refactor(tasks): improve data processing for Excel migration
  - separate logic for CustomerData and Transactions sheets
  - group transactions by CustomerID with summary statistics in migration process

🐛 fix(tasks): correct row numbering for retained headers
  - adjust row numbering logic to account for existing headers when saving new data
</commit_message>
<xml_diff>
--- a/examples/data/test_output.xlsx
+++ b/examples/data/test_output.xlsx
@@ -432,14 +432,471 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A2:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CUST0003</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>928.3100000000001</v>
+      </c>
+      <c r="D2" t="n">
+        <v>309.4366666666667</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2023-05-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CUST0006</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>665.53</v>
+      </c>
+      <c r="D3" t="n">
+        <v>332.765</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CUST0012</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1309.43</v>
+      </c>
+      <c r="D4" t="n">
+        <v>327.3575</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2023-12-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CUST0011</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>690.4100000000001</v>
+      </c>
+      <c r="D5" t="n">
+        <v>345.205</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2023-11-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CUST0018</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2080.15</v>
+      </c>
+      <c r="D6" t="n">
+        <v>520.0375</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2023-10-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CUST0014</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1303.51</v>
+      </c>
+      <c r="D7" t="n">
+        <v>651.755</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2023-07-06 00:00:00</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CUST0019</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1867.5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>466.875</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2023-09-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CUST0017</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" t="n">
+        <v>982.72</v>
+      </c>
+      <c r="D9" t="n">
+        <v>327.5733333333333</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2023-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CUST0002</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>395.94</v>
+      </c>
+      <c r="D10" t="n">
+        <v>197.97</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-05-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CUST0007</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1438.42</v>
+      </c>
+      <c r="D11" t="n">
+        <v>479.4733333333334</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CUST0001</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3001.88</v>
+      </c>
+      <c r="D12" t="n">
+        <v>500.3133333333333</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-12-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CUST0013</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1597.17</v>
+      </c>
+      <c r="D13" t="n">
+        <v>532.39</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-10-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CUST0005</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1079.01</v>
+      </c>
+      <c r="D14" t="n">
+        <v>539.505</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-09-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CUST0010</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="n">
+        <v>261.55</v>
+      </c>
+      <c r="D15" t="n">
+        <v>130.775</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-06-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CUST0004</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="n">
+        <v>820.0700000000001</v>
+      </c>
+      <c r="D16" t="n">
+        <v>273.3566666666667</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2023-11-29 00:00:00</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CUST0020</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1377.66</v>
+      </c>
+      <c r="D17" t="n">
+        <v>688.83</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023-07-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CUST0008</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="D18" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-06-07 00:00:00</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CUST0009</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="D19" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-03-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CUST0016</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="D20" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2023-04-10 00:00:00</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
♻️ refactor(engine): improve rule handling by sheet type   - optimize rule generation based on specific sheet types   - handle direct mappings and transformations efficiently
🔧 chore(logging): enhance logging for data processing
  - add detailed logging for better traceability during sheet data save operations
  - log each step and data written to Excel sheets

🔧 chore(data): restructure field mapping rules in JSON
  - reorder field mapping rules for consistency and clarity
  - replace calculation types with direct mappings where applicable

📦 build(examples): update test output Excel file content
  - modify test output file to reflect updated rule configurations and changes in data processing logic
</commit_message>
<xml_diff>
--- a/examples/data/test_output.xlsx
+++ b/examples/data/test_output.xlsx
@@ -414,14 +414,575 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A2:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CUST0001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>FirstName1 LastName1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>customer1@example.com</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>476</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2023-10-20 00:00:00</t>
+        </is>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CUST0002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>FirstName2 LastName2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>customer2@example.com</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>725</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2023-02-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CUST0003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FirstName3 LastName3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>customer3@example.com</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>481</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2023-10-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CUST0004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>FirstName4 LastName4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>customer4@example.com</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>761</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2023-01-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CUST0005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>FirstName5 LastName5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>customer5@example.com</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>595</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2023-07-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CUST0006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FirstName6 LastName6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>customer6@example.com</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>458</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2023-11-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CUST0007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>FirstName7 LastName7</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>customer7@example.com</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>581</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2023-07-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CUST0008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>FirstName8 LastName8</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>customer8@example.com</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>733</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2023-02-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CUST0009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>FirstName9 LastName9</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>customer9@example.com</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>489</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-10-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CUST0010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>FirstName10 LastName10</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>customer10@example.com</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>602</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CUST0011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>FirstName11 LastName11</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>customer11@example.com</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>703</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-03-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CUST0012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>FirstName12 LastName12</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>customer12@example.com</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>702</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-03-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CUST0013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FirstName13 LastName13</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>customer13@example.com</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>668</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-04-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CUST0014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FirstName14 LastName14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>customer14@example.com</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>594</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-07-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CUST0015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FirstName15 LastName15</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>customer15@example.com</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>409</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2024-01-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CUST0016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>FirstName16 LastName16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>customer16@example.com</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>448</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023-12-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CUST0017</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FirstName17 LastName17</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>customer17@example.com</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>714</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-03-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CUST0018</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FirstName18 LastName18</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>customer18@example.com</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>698</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-03-26 00:00:00</t>
+        </is>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CUST0019</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>FirstName19 LastName19</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>customer19@example.com</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>727</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2023-02-20 00:00:00</t>
+        </is>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CUST0020</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FirstName20 LastName20</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>customer20@example.com</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>425</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -432,7 +993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F20"/>
+  <dimension ref="A2:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -896,6 +1457,918 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CUST0003</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" t="n">
+        <v>928.3100000000001</v>
+      </c>
+      <c r="D21" t="n">
+        <v>309.4366666666667</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2023-05-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CUST0006</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" t="n">
+        <v>665.53</v>
+      </c>
+      <c r="D22" t="n">
+        <v>332.765</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CUST0012</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1309.43</v>
+      </c>
+      <c r="D23" t="n">
+        <v>327.3575</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2023-12-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CUST0011</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" t="n">
+        <v>690.4100000000001</v>
+      </c>
+      <c r="D24" t="n">
+        <v>345.205</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2023-11-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CUST0018</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2080.15</v>
+      </c>
+      <c r="D25" t="n">
+        <v>520.0375</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2023-10-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CUST0014</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1303.51</v>
+      </c>
+      <c r="D26" t="n">
+        <v>651.755</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2023-07-06 00:00:00</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CUST0019</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1867.5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>466.875</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2023-09-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CUST0017</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" t="n">
+        <v>982.72</v>
+      </c>
+      <c r="D28" t="n">
+        <v>327.5733333333333</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2023-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CUST0002</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" t="n">
+        <v>395.94</v>
+      </c>
+      <c r="D29" t="n">
+        <v>197.97</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2023-05-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>CUST0007</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1438.42</v>
+      </c>
+      <c r="D30" t="n">
+        <v>479.4733333333334</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CUST0001</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>6</v>
+      </c>
+      <c r="C31" t="n">
+        <v>3001.88</v>
+      </c>
+      <c r="D31" t="n">
+        <v>500.3133333333333</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2023-12-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CUST0013</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1597.17</v>
+      </c>
+      <c r="D32" t="n">
+        <v>532.39</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2023-10-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CUST0005</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1079.01</v>
+      </c>
+      <c r="D33" t="n">
+        <v>539.505</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2023-09-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CUST0010</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" t="n">
+        <v>261.55</v>
+      </c>
+      <c r="D34" t="n">
+        <v>130.775</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2023-06-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CUST0004</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" t="n">
+        <v>820.0700000000001</v>
+      </c>
+      <c r="D35" t="n">
+        <v>273.3566666666667</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2023-11-29 00:00:00</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CUST0020</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1377.66</v>
+      </c>
+      <c r="D36" t="n">
+        <v>688.83</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2023-07-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CUST0008</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="D37" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2023-06-07 00:00:00</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CUST0009</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="D38" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2023-03-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CUST0016</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="D39" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2023-04-10 00:00:00</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CUST0003</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" t="n">
+        <v>928.3100000000001</v>
+      </c>
+      <c r="D40" t="n">
+        <v>309.4366666666667</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2023-05-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CUST0006</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" t="n">
+        <v>665.53</v>
+      </c>
+      <c r="D41" t="n">
+        <v>332.765</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CUST0012</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>4</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1309.43</v>
+      </c>
+      <c r="D42" t="n">
+        <v>327.3575</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2023-12-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CUST0011</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" t="n">
+        <v>690.4100000000001</v>
+      </c>
+      <c r="D43" t="n">
+        <v>345.205</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2023-11-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CUST0018</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>4</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2080.15</v>
+      </c>
+      <c r="D44" t="n">
+        <v>520.0375</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2023-10-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CUST0014</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1303.51</v>
+      </c>
+      <c r="D45" t="n">
+        <v>651.755</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2023-07-06 00:00:00</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CUST0019</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1867.5</v>
+      </c>
+      <c r="D46" t="n">
+        <v>466.875</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2023-09-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CUST0017</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>3</v>
+      </c>
+      <c r="C47" t="n">
+        <v>982.72</v>
+      </c>
+      <c r="D47" t="n">
+        <v>327.5733333333333</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2023-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CUST0002</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" t="n">
+        <v>395.94</v>
+      </c>
+      <c r="D48" t="n">
+        <v>197.97</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2023-05-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CUST0007</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1438.42</v>
+      </c>
+      <c r="D49" t="n">
+        <v>479.4733333333334</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CUST0001</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>6</v>
+      </c>
+      <c r="C50" t="n">
+        <v>3001.88</v>
+      </c>
+      <c r="D50" t="n">
+        <v>500.3133333333333</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2023-12-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CUST0013</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1597.17</v>
+      </c>
+      <c r="D51" t="n">
+        <v>532.39</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2023-10-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CUST0005</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1079.01</v>
+      </c>
+      <c r="D52" t="n">
+        <v>539.505</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2023-09-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CUST0010</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" t="n">
+        <v>261.55</v>
+      </c>
+      <c r="D53" t="n">
+        <v>130.775</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2023-06-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CUST0004</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>3</v>
+      </c>
+      <c r="C54" t="n">
+        <v>820.0700000000001</v>
+      </c>
+      <c r="D54" t="n">
+        <v>273.3566666666667</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2023-11-29 00:00:00</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>CUST0020</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1377.66</v>
+      </c>
+      <c r="D55" t="n">
+        <v>688.83</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2023-07-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CUST0008</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="D56" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2023-06-07 00:00:00</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CUST0009</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="D57" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2023-03-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CUST0016</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="D58" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2023-04-10 00:00:00</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✨ feat(plugins): implement Excel migration plugin system
- add initial implementation of Excel migration plugins with various formula executors and transformation handlers
- introduce a plugin registry to manage and retrieve formula executors and transformation handlers

♻️ refactor(executor): update rule executor to use plugins

- integrate plugin system with rule executor for formula execution and transformation
- ensure validation and execution methods utilize registered plugins

🐛 fix(tasks): correct data writing in task-based processor

- fix the loop for writing data to ensure correct values are assigned from data dictionary
- improve logging within the data writing process

⚡️ perf(executor): optimize rule execution with async validation

- add async validation of rules to improve efficiency within rule execution process
</commit_message>
<xml_diff>
--- a/examples/data/test_output.xlsx
+++ b/examples/data/test_output.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F21"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,6 +422,38 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>CustomerID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>FullName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>DaysSinceRegistration</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>LastLoginDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>IsActive</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
@@ -979,6 +1011,566 @@
         </is>
       </c>
       <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CUST0001</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>FirstName1 LastName1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>customer1@example.com</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>476</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2023-10-20 00:00:00</t>
+        </is>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CUST0002</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FirstName2 LastName2</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>customer2@example.com</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>725</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2023-02-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CUST0003</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>FirstName3 LastName3</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>customer3@example.com</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>481</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2023-10-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CUST0004</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>FirstName4 LastName4</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>customer4@example.com</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>761</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2023-01-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CUST0005</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>FirstName5 LastName5</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>customer5@example.com</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>595</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2023-07-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CUST0006</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>FirstName6 LastName6</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>customer6@example.com</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>458</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2023-11-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CUST0007</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>FirstName7 LastName7</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>customer7@example.com</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>581</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2023-07-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CUST0008</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>FirstName8 LastName8</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>customer8@example.com</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>733</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2023-02-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>CUST0009</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>FirstName9 LastName9</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>customer9@example.com</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>489</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2023-10-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CUST0010</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>FirstName10 LastName10</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>customer10@example.com</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>602</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2023-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CUST0011</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>FirstName11 LastName11</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>customer11@example.com</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>703</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2023-03-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CUST0012</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>FirstName12 LastName12</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>customer12@example.com</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>702</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2023-03-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CUST0013</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>FirstName13 LastName13</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>customer13@example.com</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>668</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2023-04-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CUST0014</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>FirstName14 LastName14</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>customer14@example.com</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>594</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2023-07-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CUST0015</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>FirstName15 LastName15</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>customer15@example.com</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>409</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2024-01-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CUST0016</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FirstName16 LastName16</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>customer16@example.com</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>448</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2023-12-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CUST0017</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>FirstName17 LastName17</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>customer17@example.com</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>714</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2023-03-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CUST0018</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>FirstName18 LastName18</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>customer18@example.com</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>698</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2023-03-26 00:00:00</t>
+        </is>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CUST0019</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>FirstName19 LastName19</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>customer19@example.com</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>727</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2023-02-20 00:00:00</t>
+        </is>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CUST0020</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>FirstName20 LastName20</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>customer20@example.com</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>425</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="F41" t="b">
         <v>0</v>
       </c>
     </row>
@@ -993,7 +1585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F58"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1001,6 +1593,38 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>CustomerID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TransactionCount</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>TotalAmount</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>AverageAmount</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>LastTransactionDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>SuccessRate</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
@@ -2366,6 +2990,462 @@
         </is>
       </c>
       <c r="F58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CUST0003</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>3</v>
+      </c>
+      <c r="C59" t="n">
+        <v>928.3100000000001</v>
+      </c>
+      <c r="D59" t="n">
+        <v>309.4366666666667</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2023-05-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CUST0006</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" t="n">
+        <v>665.53</v>
+      </c>
+      <c r="D60" t="n">
+        <v>332.765</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>CUST0012</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1309.43</v>
+      </c>
+      <c r="D61" t="n">
+        <v>327.3575</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2023-12-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>CUST0011</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>2</v>
+      </c>
+      <c r="C62" t="n">
+        <v>690.4100000000001</v>
+      </c>
+      <c r="D62" t="n">
+        <v>345.205</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2023-11-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>CUST0018</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>4</v>
+      </c>
+      <c r="C63" t="n">
+        <v>2080.15</v>
+      </c>
+      <c r="D63" t="n">
+        <v>520.0375</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2023-10-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>CUST0014</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1303.51</v>
+      </c>
+      <c r="D64" t="n">
+        <v>651.755</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2023-07-06 00:00:00</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>CUST0019</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1867.5</v>
+      </c>
+      <c r="D65" t="n">
+        <v>466.875</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2023-09-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>CUST0017</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>3</v>
+      </c>
+      <c r="C66" t="n">
+        <v>982.72</v>
+      </c>
+      <c r="D66" t="n">
+        <v>327.5733333333333</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2023-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>CUST0002</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" t="n">
+        <v>395.94</v>
+      </c>
+      <c r="D67" t="n">
+        <v>197.97</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2023-05-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>CUST0007</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>3</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1438.42</v>
+      </c>
+      <c r="D68" t="n">
+        <v>479.4733333333334</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>CUST0001</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>6</v>
+      </c>
+      <c r="C69" t="n">
+        <v>3001.88</v>
+      </c>
+      <c r="D69" t="n">
+        <v>500.3133333333333</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2023-12-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>CUST0013</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>3</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1597.17</v>
+      </c>
+      <c r="D70" t="n">
+        <v>532.39</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2023-10-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>CUST0005</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1079.01</v>
+      </c>
+      <c r="D71" t="n">
+        <v>539.505</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2023-09-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>CUST0010</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>2</v>
+      </c>
+      <c r="C72" t="n">
+        <v>261.55</v>
+      </c>
+      <c r="D72" t="n">
+        <v>130.775</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2023-06-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>CUST0004</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>3</v>
+      </c>
+      <c r="C73" t="n">
+        <v>820.0700000000001</v>
+      </c>
+      <c r="D73" t="n">
+        <v>273.3566666666667</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2023-11-29 00:00:00</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>CUST0020</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>2</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1377.66</v>
+      </c>
+      <c r="D74" t="n">
+        <v>688.83</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2023-07-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>CUST0008</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="D75" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2023-06-07 00:00:00</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>CUST0009</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="D76" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2023-03-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>CUST0016</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="D77" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2023-04-10 00:00:00</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📝 docs(README): add plugin system documentation
- introduce plugin-based rule execution with extensible formula executors
- explain modular design and SOLID principles for custom transformations
- expand documentation with examples for formula executors and transformation handlers

🔧 chore(examples): update test_output.xlsx

- update binary file for test output in examples/data directory
</commit_message>
<xml_diff>
--- a/examples/data/test_output.xlsx
+++ b/examples/data/test_output.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1571,6 +1571,566 @@
         </is>
       </c>
       <c r="F41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CUST0001</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>FirstName1 LastName1</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>customer1@example.com</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>476</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2023-10-20 00:00:00</t>
+        </is>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CUST0002</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>FirstName2 LastName2</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>customer2@example.com</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>725</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2023-02-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CUST0003</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>FirstName3 LastName3</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>customer3@example.com</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>481</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2023-10-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CUST0004</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>FirstName4 LastName4</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>customer4@example.com</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>761</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2023-01-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CUST0005</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>FirstName5 LastName5</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>customer5@example.com</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>595</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2023-07-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CUST0006</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>FirstName6 LastName6</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>customer6@example.com</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>458</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2023-11-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CUST0007</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>FirstName7 LastName7</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>customer7@example.com</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>581</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2023-07-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CUST0008</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>FirstName8 LastName8</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>customer8@example.com</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>733</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2023-02-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CUST0009</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>FirstName9 LastName9</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>customer9@example.com</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>489</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2023-10-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CUST0010</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>FirstName10 LastName10</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>customer10@example.com</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>602</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2023-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CUST0011</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>FirstName11 LastName11</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>customer11@example.com</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>703</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2023-03-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CUST0012</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>FirstName12 LastName12</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>customer12@example.com</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>702</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2023-03-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CUST0013</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>FirstName13 LastName13</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>customer13@example.com</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>668</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2023-04-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>CUST0014</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>FirstName14 LastName14</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>customer14@example.com</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>594</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2023-07-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CUST0015</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>FirstName15 LastName15</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>customer15@example.com</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>409</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2024-01-08 00:00:00</t>
+        </is>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CUST0016</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>FirstName16 LastName16</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>customer16@example.com</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>448</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2023-12-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CUST0017</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>FirstName17 LastName17</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>customer17@example.com</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>714</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2023-03-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CUST0018</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>FirstName18 LastName18</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>customer18@example.com</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>698</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2023-03-26 00:00:00</t>
+        </is>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CUST0019</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>FirstName19 LastName19</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>customer19@example.com</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>727</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2023-02-20 00:00:00</t>
+        </is>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>CUST0020</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>FirstName20 LastName20</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>customer20@example.com</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>425</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="F61" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1585,7 +2145,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3449,6 +4009,462 @@
         <v>1</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>CUST0003</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>3</v>
+      </c>
+      <c r="C78" t="n">
+        <v>928.3100000000001</v>
+      </c>
+      <c r="D78" t="n">
+        <v>309.4366666666667</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2023-05-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>CUST0006</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>2</v>
+      </c>
+      <c r="C79" t="n">
+        <v>665.53</v>
+      </c>
+      <c r="D79" t="n">
+        <v>332.765</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>CUST0012</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>4</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1309.43</v>
+      </c>
+      <c r="D80" t="n">
+        <v>327.3575</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2023-12-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>CUST0011</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>2</v>
+      </c>
+      <c r="C81" t="n">
+        <v>690.4100000000001</v>
+      </c>
+      <c r="D81" t="n">
+        <v>345.205</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2023-11-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>CUST0018</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>4</v>
+      </c>
+      <c r="C82" t="n">
+        <v>2080.15</v>
+      </c>
+      <c r="D82" t="n">
+        <v>520.0375</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2023-10-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>CUST0014</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>2</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1303.51</v>
+      </c>
+      <c r="D83" t="n">
+        <v>651.755</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2023-07-06 00:00:00</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>CUST0019</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>4</v>
+      </c>
+      <c r="C84" t="n">
+        <v>1867.5</v>
+      </c>
+      <c r="D84" t="n">
+        <v>466.875</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2023-09-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>CUST0017</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>3</v>
+      </c>
+      <c r="C85" t="n">
+        <v>982.72</v>
+      </c>
+      <c r="D85" t="n">
+        <v>327.5733333333333</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2023-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>CUST0002</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>2</v>
+      </c>
+      <c r="C86" t="n">
+        <v>395.94</v>
+      </c>
+      <c r="D86" t="n">
+        <v>197.97</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2023-05-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>CUST0007</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>3</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1438.42</v>
+      </c>
+      <c r="D87" t="n">
+        <v>479.4733333333334</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2023-06-27 00:00:00</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>CUST0001</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>6</v>
+      </c>
+      <c r="C88" t="n">
+        <v>3001.88</v>
+      </c>
+      <c r="D88" t="n">
+        <v>500.3133333333333</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2023-12-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>CUST0013</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>3</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1597.17</v>
+      </c>
+      <c r="D89" t="n">
+        <v>532.39</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2023-10-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>CUST0005</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>2</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1079.01</v>
+      </c>
+      <c r="D90" t="n">
+        <v>539.505</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2023-09-19 00:00:00</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>CUST0010</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>2</v>
+      </c>
+      <c r="C91" t="n">
+        <v>261.55</v>
+      </c>
+      <c r="D91" t="n">
+        <v>130.775</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2023-06-13 00:00:00</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>CUST0004</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>3</v>
+      </c>
+      <c r="C92" t="n">
+        <v>820.0700000000001</v>
+      </c>
+      <c r="D92" t="n">
+        <v>273.3566666666667</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2023-11-29 00:00:00</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>CUST0020</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>2</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1377.66</v>
+      </c>
+      <c r="D93" t="n">
+        <v>688.83</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2023-07-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>CUST0008</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>1</v>
+      </c>
+      <c r="C94" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="D94" t="n">
+        <v>330.22</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2023-06-07 00:00:00</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>CUST0009</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="D95" t="n">
+        <v>665.04</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>2023-03-25 00:00:00</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>CUST0016</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="D96" t="n">
+        <v>616.3</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>2023-04-10 00:00:00</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>